<commit_message>
Wait for creating led-show module.
Signed-off-by: dtysky <dtysky@outlook.com>
</commit_message>
<xml_diff>
--- a/CPU_ON_BOARD/buttons_function.xlsx
+++ b/CPU_ON_BOARD/buttons_function.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -551,18 +551,19 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="117" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="1" t="s">
+    <row r="10" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="13" spans="1:14" ht="117" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>